<commit_message>
alltoall table is created
</commit_message>
<xml_diff>
--- a/MVAPICH/Results/Analysis/Local/SecureAlltoall/10rep-NS-AlltoAll-MVAPICH.xlsx
+++ b/MVAPICH/Results/Analysis/Local/SecureAlltoall/10rep-NS-AlltoAll-MVAPICH.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="34">
   <si>
     <t xml:space="preserve">8 Nodes - 128 Ranks - Block</t>
   </si>
@@ -137,6 +137,9 @@
     <t xml:space="preserve">Naive-CHS</t>
   </si>
   <si>
+    <t xml:space="preserve">e</t>
+  </si>
+  <si>
     <t xml:space="preserve">Naive-SD</t>
   </si>
 </sst>
@@ -144,9 +147,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="0.00"/>
+    <numFmt numFmtId="166" formatCode="0.00E+00"/>
   </numFmts>
   <fonts count="12">
     <font>
@@ -304,7 +308,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -386,6 +390,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -476,7 +484,7 @@
       <selection pane="topLeft" activeCell="G38" activeCellId="0" sqref="G38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.78515625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.8046875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="69" min="1" style="1" width="14.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1020" style="2" width="11.52"/>
@@ -2361,10 +2369,10 @@
   <dimension ref="A1:P1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H29" activeCellId="0" sqref="H29"/>
+      <selection pane="topLeft" activeCell="L35" activeCellId="0" sqref="L35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.78515625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.8046875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="14.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="22.88"/>
@@ -2501,7 +2509,7 @@
       <c r="L5" s="21" t="n">
         <v>26.068</v>
       </c>
-      <c r="M5" s="21" t="n">
+      <c r="M5" s="22" t="n">
         <f aca="false">100*(D5-B5)/B5</f>
         <v>821.720116618076</v>
       </c>
@@ -2509,11 +2517,11 @@
         <f aca="false">K5</f>
         <v>33.67</v>
       </c>
-      <c r="O5" s="21" t="n">
+      <c r="O5" s="22" t="n">
         <f aca="false">100*(N5-L5)/L5</f>
         <v>29.1621911922664</v>
       </c>
-      <c r="P5" s="21" t="s">
+      <c r="P5" s="22" t="s">
         <v>30</v>
       </c>
     </row>
@@ -2555,7 +2563,7 @@
       <c r="L6" s="21" t="n">
         <v>25.914</v>
       </c>
-      <c r="M6" s="21" t="n">
+      <c r="M6" s="22" t="n">
         <f aca="false">100*(D6-B6)/B6</f>
         <v>827.660723933009</v>
       </c>
@@ -2563,11 +2571,11 @@
         <f aca="false">K6</f>
         <v>35.55</v>
       </c>
-      <c r="O6" s="21" t="n">
+      <c r="O6" s="22" t="n">
         <f aca="false">100*(N6-L6)/L6</f>
         <v>37.1845334568187</v>
       </c>
-      <c r="P6" s="21" t="s">
+      <c r="P6" s="22" t="s">
         <v>30</v>
       </c>
     </row>
@@ -2609,7 +2617,7 @@
       <c r="L7" s="21" t="n">
         <v>28.38</v>
       </c>
-      <c r="M7" s="21" t="n">
+      <c r="M7" s="22" t="n">
         <f aca="false">100*(D7-B7)/B7</f>
         <v>752.508809020437</v>
       </c>
@@ -2617,11 +2625,11 @@
         <f aca="false">K7</f>
         <v>36.298</v>
       </c>
-      <c r="O7" s="21" t="n">
+      <c r="O7" s="22" t="n">
         <f aca="false">100*(N7-L7)/L7</f>
         <v>27.8999295278365</v>
       </c>
-      <c r="P7" s="21" t="s">
+      <c r="P7" s="22" t="s">
         <v>30</v>
       </c>
     </row>
@@ -2663,7 +2671,7 @@
       <c r="L8" s="21" t="n">
         <v>29.368</v>
       </c>
-      <c r="M8" s="21" t="n">
+      <c r="M8" s="22" t="n">
         <f aca="false">100*(D8-B8)/B8</f>
         <v>744.197766276219</v>
       </c>
@@ -2671,11 +2679,11 @@
         <f aca="false">K8</f>
         <v>38.478</v>
       </c>
-      <c r="O8" s="21" t="n">
+      <c r="O8" s="22" t="n">
         <f aca="false">100*(N8-L8)/L8</f>
         <v>31.0201579950967</v>
       </c>
-      <c r="P8" s="21" t="s">
+      <c r="P8" s="22" t="s">
         <v>30</v>
       </c>
     </row>
@@ -2717,7 +2725,7 @@
       <c r="L9" s="21" t="n">
         <v>30.81</v>
       </c>
-      <c r="M9" s="21" t="n">
+      <c r="M9" s="22" t="n">
         <f aca="false">100*(D9-B9)/B9</f>
         <v>684.297306069458</v>
       </c>
@@ -2725,11 +2733,11 @@
         <f aca="false">K9</f>
         <v>37.032</v>
       </c>
-      <c r="O9" s="21" t="n">
+      <c r="O9" s="22" t="n">
         <f aca="false">100*(N9-L9)/L9</f>
         <v>20.1947419668939</v>
       </c>
-      <c r="P9" s="21" t="s">
+      <c r="P9" s="22" t="s">
         <v>31</v>
       </c>
     </row>
@@ -2771,7 +2779,7 @@
       <c r="L10" s="21" t="n">
         <v>33.992</v>
       </c>
-      <c r="M10" s="21" t="n">
+      <c r="M10" s="22" t="n">
         <f aca="false">100*(D10-B10)/B10</f>
         <v>629.595198870323</v>
       </c>
@@ -2779,11 +2787,11 @@
         <f aca="false">K10</f>
         <v>40.932</v>
       </c>
-      <c r="O10" s="21" t="n">
+      <c r="O10" s="22" t="n">
         <f aca="false">100*(N10-L10)/L10</f>
         <v>20.4165686043775</v>
       </c>
-      <c r="P10" s="21" t="s">
+      <c r="P10" s="22" t="s">
         <v>31</v>
       </c>
     </row>
@@ -2825,7 +2833,7 @@
       <c r="L11" s="21" t="n">
         <v>42.866</v>
       </c>
-      <c r="M11" s="21" t="n">
+      <c r="M11" s="22" t="n">
         <f aca="false">100*(D11-B11)/B11</f>
         <v>540.297671814492</v>
       </c>
@@ -2833,11 +2841,11 @@
         <f aca="false">K11</f>
         <v>48.498</v>
       </c>
-      <c r="O11" s="21" t="n">
+      <c r="O11" s="22" t="n">
         <f aca="false">100*(N11-L11)/L11</f>
         <v>13.1386180189427</v>
       </c>
-      <c r="P11" s="21" t="s">
+      <c r="P11" s="22" t="s">
         <v>31</v>
       </c>
     </row>
@@ -2869,8 +2877,8 @@
       <c r="I12" s="19" t="n">
         <v>800.2</v>
       </c>
-      <c r="J12" s="19" t="n">
-        <v>72.208</v>
+      <c r="J12" s="19" t="s">
+        <v>32</v>
       </c>
       <c r="K12" s="20" t="n">
         <f aca="false">MIN(D12:J12)</f>
@@ -2879,7 +2887,7 @@
       <c r="L12" s="21" t="n">
         <v>64.904</v>
       </c>
-      <c r="M12" s="21" t="n">
+      <c r="M12" s="22" t="n">
         <f aca="false">100*(D12-B12)/B12</f>
         <v>345.072722790583</v>
       </c>
@@ -2887,11 +2895,11 @@
         <f aca="false">K12</f>
         <v>63.31</v>
       </c>
-      <c r="O12" s="21" t="n">
+      <c r="O12" s="22" t="n">
         <f aca="false">100*(N12-L12)/L12</f>
         <v>-2.45593491926537</v>
       </c>
-      <c r="P12" s="21" t="s">
+      <c r="P12" s="22" t="s">
         <v>31</v>
       </c>
     </row>
@@ -2933,7 +2941,7 @@
       <c r="L13" s="21" t="n">
         <v>158.05</v>
       </c>
-      <c r="M13" s="21" t="n">
+      <c r="M13" s="22" t="n">
         <f aca="false">100*(D13-B13)/B13</f>
         <v>153.955077507118</v>
       </c>
@@ -2941,11 +2949,11 @@
         <f aca="false">K13</f>
         <v>101.328</v>
       </c>
-      <c r="O13" s="21" t="n">
+      <c r="O13" s="22" t="n">
         <f aca="false">100*(N13-L13)/L13</f>
         <v>-35.888642834546</v>
       </c>
-      <c r="P13" s="21" t="s">
+      <c r="P13" s="22" t="s">
         <v>31</v>
       </c>
     </row>
@@ -2987,7 +2995,7 @@
       <c r="L14" s="21" t="n">
         <v>262</v>
       </c>
-      <c r="M14" s="21" t="n">
+      <c r="M14" s="22" t="n">
         <f aca="false">100*(D14-B14)/B14</f>
         <v>99.4503816793893</v>
       </c>
@@ -2995,11 +3003,11 @@
         <f aca="false">K14</f>
         <v>171.57</v>
       </c>
-      <c r="O14" s="21" t="n">
+      <c r="O14" s="22" t="n">
         <f aca="false">100*(N14-L14)/L14</f>
         <v>-34.5152671755725</v>
       </c>
-      <c r="P14" s="21" t="s">
+      <c r="P14" s="22" t="s">
         <v>31</v>
       </c>
     </row>
@@ -3041,7 +3049,7 @@
       <c r="L15" s="21" t="n">
         <v>507.146</v>
       </c>
-      <c r="M15" s="21" t="n">
+      <c r="M15" s="22" t="n">
         <f aca="false">100*(D15-B15)/B15</f>
         <v>58.3145681914084</v>
       </c>
@@ -3049,11 +3057,11 @@
         <f aca="false">K15</f>
         <v>378.678</v>
       </c>
-      <c r="O15" s="21" t="n">
+      <c r="O15" s="22" t="n">
         <f aca="false">100*(N15-L15)/L15</f>
         <v>-25.3315613255354</v>
       </c>
-      <c r="P15" s="21" t="s">
+      <c r="P15" s="22" t="s">
         <v>31</v>
       </c>
     </row>
@@ -3095,7 +3103,7 @@
       <c r="L16" s="21" t="n">
         <v>427.78</v>
       </c>
-      <c r="M16" s="21" t="n">
+      <c r="M16" s="22" t="n">
         <f aca="false">100*(E16-B16)/B16</f>
         <v>69.1771471317032</v>
       </c>
@@ -3103,12 +3111,12 @@
         <f aca="false">K16</f>
         <v>723.706</v>
       </c>
-      <c r="O16" s="21" t="n">
+      <c r="O16" s="22" t="n">
         <f aca="false">100*(N16-L16)/L16</f>
         <v>69.1771471317032</v>
       </c>
-      <c r="P16" s="21" t="s">
-        <v>32</v>
+      <c r="P16" s="22" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3149,7 +3157,7 @@
       <c r="L17" s="21" t="n">
         <v>752.658</v>
       </c>
-      <c r="M17" s="21" t="n">
+      <c r="M17" s="22" t="n">
         <f aca="false">100*(E17-B17)/B17</f>
         <v>67.1672924488945</v>
       </c>
@@ -3157,12 +3165,12 @@
         <f aca="false">K17</f>
         <v>1258.198</v>
       </c>
-      <c r="O17" s="21" t="n">
+      <c r="O17" s="22" t="n">
         <f aca="false">100*(N17-L17)/L17</f>
         <v>67.1672924488945</v>
       </c>
-      <c r="P17" s="21" t="s">
-        <v>32</v>
+      <c r="P17" s="22" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3203,7 +3211,7 @@
       <c r="L18" s="21" t="n">
         <v>1572.042</v>
       </c>
-      <c r="M18" s="21" t="n">
+      <c r="M18" s="22" t="n">
         <f aca="false">100*(E18-B18)/B18</f>
         <v>60.586930883526</v>
       </c>
@@ -3211,12 +3219,12 @@
         <f aca="false">K18</f>
         <v>2524.494</v>
       </c>
-      <c r="O18" s="21" t="n">
+      <c r="O18" s="22" t="n">
         <f aca="false">100*(N18-L18)/L18</f>
         <v>60.586930883526</v>
       </c>
-      <c r="P18" s="21" t="s">
-        <v>32</v>
+      <c r="P18" s="22" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3257,7 +3265,7 @@
       <c r="L19" s="21" t="n">
         <v>3950.292</v>
       </c>
-      <c r="M19" s="21" t="n">
+      <c r="M19" s="22" t="n">
         <f aca="false">100*(E19-B19)/B19</f>
         <v>48.9163839027596</v>
       </c>
@@ -3265,12 +3273,12 @@
         <f aca="false">K19</f>
         <v>5882.632</v>
       </c>
-      <c r="O19" s="21" t="n">
+      <c r="O19" s="22" t="n">
         <f aca="false">100*(N19-L19)/L19</f>
         <v>48.9163839027596</v>
       </c>
-      <c r="P19" s="21" t="s">
-        <v>32</v>
+      <c r="P19" s="22" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3311,7 +3319,7 @@
       <c r="L20" s="21" t="n">
         <v>7904.346</v>
       </c>
-      <c r="M20" s="21" t="n">
+      <c r="M20" s="22" t="n">
         <f aca="false">100*(E20-B20)/B20</f>
         <v>51.3793298016054</v>
       </c>
@@ -3319,12 +3327,12 @@
         <f aca="false">K20</f>
         <v>11965.546</v>
       </c>
-      <c r="O20" s="21" t="n">
+      <c r="O20" s="22" t="n">
         <f aca="false">100*(N20-L20)/L20</f>
         <v>51.3793298016054</v>
       </c>
-      <c r="P20" s="21" t="s">
-        <v>32</v>
+      <c r="P20" s="22" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3365,7 +3373,7 @@
       <c r="L21" s="21" t="n">
         <v>11658.544</v>
       </c>
-      <c r="M21" s="21" t="n">
+      <c r="M21" s="22" t="n">
         <f aca="false">100*(E21-B21)/B21</f>
         <v>75.1731605593289</v>
       </c>
@@ -3373,12 +3381,12 @@
         <f aca="false">K21</f>
         <v>20422.64</v>
       </c>
-      <c r="O21" s="21" t="n">
+      <c r="O21" s="22" t="n">
         <f aca="false">100*(N21-L21)/L21</f>
         <v>75.1731605593289</v>
       </c>
-      <c r="P21" s="21" t="s">
-        <v>32</v>
+      <c r="P21" s="22" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3419,7 +3427,7 @@
       <c r="L22" s="21" t="n">
         <v>22215.154</v>
       </c>
-      <c r="M22" s="21" t="n">
+      <c r="M22" s="22" t="n">
         <f aca="false">100*(E22-B22)/B22</f>
         <v>77.5548978863707</v>
       </c>
@@ -3427,12 +3435,12 @@
         <f aca="false">K22</f>
         <v>39444.094</v>
       </c>
-      <c r="O22" s="21" t="n">
+      <c r="O22" s="22" t="n">
         <f aca="false">100*(N22-L22)/L22</f>
         <v>77.5548978863707</v>
       </c>
-      <c r="P22" s="21" t="s">
-        <v>32</v>
+      <c r="P22" s="22" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3473,7 +3481,7 @@
       <c r="L23" s="21" t="n">
         <v>43565.738</v>
       </c>
-      <c r="M23" s="21" t="n">
+      <c r="M23" s="22" t="n">
         <f aca="false">100*(E23-B23)/B23</f>
         <v>78.2602282555159</v>
       </c>
@@ -3481,12 +3489,12 @@
         <f aca="false">K23</f>
         <v>77660.384</v>
       </c>
-      <c r="O23" s="21" t="n">
+      <c r="O23" s="22" t="n">
         <f aca="false">100*(N23-L23)/L23</f>
         <v>78.2602282555159</v>
       </c>
-      <c r="P23" s="21" t="s">
-        <v>32</v>
+      <c r="P23" s="22" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5155,7 +5163,7 @@
       <selection pane="topLeft" activeCell="M23" activeCellId="0" sqref="M23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.78515625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.8046875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="69" min="1" style="1" width="14.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1020" style="2" width="11.52"/>
@@ -7043,7 +7051,7 @@
       <selection pane="topLeft" activeCell="M23" activeCellId="0" sqref="M23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.78515625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.8046875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="69" min="1" style="1" width="14.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1020" style="2" width="11.52"/>
@@ -8931,7 +8939,7 @@
       <selection pane="topLeft" activeCell="M23" activeCellId="0" sqref="M23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.78515625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.8046875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="69" min="1" style="1" width="14.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1020" style="2" width="11.52"/>
@@ -10819,7 +10827,7 @@
       <selection pane="topLeft" activeCell="M23" activeCellId="0" sqref="M23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.78515625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.8046875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="69" min="1" style="1" width="14.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1020" style="2" width="11.52"/>
@@ -12707,7 +12715,7 @@
       <selection pane="topLeft" activeCell="M23" activeCellId="0" sqref="M23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.78515625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.8046875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="69" min="1" style="1" width="14.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1020" style="2" width="11.52"/>
@@ -14595,7 +14603,7 @@
       <selection pane="topLeft" activeCell="M23" activeCellId="0" sqref="M23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.78515625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.8046875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="69" min="1" style="1" width="14.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1020" style="2" width="11.52"/>
@@ -16483,7 +16491,7 @@
       <selection pane="topLeft" activeCell="M23" activeCellId="0" sqref="M23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.78515625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.8046875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="69" min="1" style="1" width="14.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1020" style="2" width="11.52"/>
@@ -18371,7 +18379,7 @@
       <selection pane="topLeft" activeCell="M23" activeCellId="0" sqref="M23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.78515625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.8046875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="69" min="1" style="1" width="14.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1020" style="2" width="11.52"/>

</xml_diff>